<commit_message>
Data Clean and Scatter Plot
</commit_message>
<xml_diff>
--- a/Data_Banks_EuroStoxx600_Euribor.xlsx
+++ b/Data_Banks_EuroStoxx600_Euribor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\Desktop\Magistrale\Esami\Regression\Project_Banks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricca\Desktop\Magistrale\Esami\Regression\Project_Banks\Work_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1740098D-0F33-49C7-984F-E859DBEB8D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA46045-3C95-4F04-982B-AC671DD3B7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A8F0B263-05CE-466E-98C0-EC382219F419}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <author>Riccardo Caruso</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{3A895AF5-8897-4C77-97FE-14F8CDC8127B}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{184A6A80-4173-4474-A5C3-0C9C83017727}">
       <text>
         <r>
           <rPr>
@@ -220,23 +220,23 @@
       <tp t="s">
         <v>Name</v>
         <stp/>
-        <stp>2</stp>
-        <stp>23740890</stp>
+        <stp>3</stp>
+        <stp>264794734</stp>
         <tr r="A1" s="3"/>
       </tp>
       <tp t="s">
         <v>Name</v>
         <stp/>
-        <stp>3</stp>
-        <stp>23740890</stp>
-        <tr r="A1" s="2"/>
+        <stp>2</stp>
+        <stp>264794734</stp>
+        <tr r="A1" s="4"/>
       </tp>
       <tp t="s">
         <v>Name</v>
         <stp/>
         <stp>1</stp>
-        <stp>23740890</stp>
-        <tr r="A1" s="4"/>
+        <stp>264794734</stp>
+        <tr r="A1" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1906,10 +1906,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="REFI_OFFICE_FUNCTION_DATA" r:id="rId1"/>
-  </customProperties>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>